<commit_message>
Just need to do some clean up
</commit_message>
<xml_diff>
--- a/Angajati.xlsx
+++ b/Angajati.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://futureworkforcecompany-my.sharepoint.com/personal/james_weller_fwfcompany_com/Documents/Documents/GitHub/REF-Revisal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://futureworkforcecompany-my.sharepoint.com/personal/patricia_ciortin_fwfcompany_com/Documents/Desktop/Internship Documentation Updated/Revisal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{F23EB0EA-9C3B-4545-A2E2-483DF48D89DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9314FC7D-B82E-4F7A-982A-31392358C9AE}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{F23EB0EA-9C3B-4545-A2E2-483DF48D89DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E11D5DE-FF49-4477-8970-334D212678A8}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="24" windowWidth="15444" windowHeight="12216" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Angajati" sheetId="1" r:id="rId1"/>
@@ -404,18 +404,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -725,674 +727,682 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="48.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.33203125" customWidth="1"/>
-    <col min="13" max="13" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.88671875" customWidth="1"/>
-    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="22.44140625" customWidth="1"/>
-    <col min="18" max="18" width="14.6640625" customWidth="1"/>
-    <col min="19" max="19" width="22.109375" customWidth="1"/>
-    <col min="20" max="20" width="14.6640625" customWidth="1"/>
-    <col min="21" max="21" width="22.44140625" customWidth="1"/>
+    <col min="9" max="9" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.28515625" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" customWidth="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="22.42578125" customWidth="1"/>
+    <col min="18" max="18" width="14.7109375" customWidth="1"/>
+    <col min="19" max="19" width="22.140625" customWidth="1"/>
+    <col min="20" max="20" width="14.7109375" customWidth="1"/>
+    <col min="21" max="21" width="22.42578125" customWidth="1"/>
     <col min="22" max="23" width="23" customWidth="1"/>
-    <col min="24" max="24" width="8.6640625" customWidth="1"/>
-    <col min="25" max="25" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.88671875" customWidth="1"/>
+    <col min="24" max="24" width="8.7109375" customWidth="1"/>
+    <col min="25" max="25" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.85546875" customWidth="1"/>
     <col min="27" max="27" width="12" customWidth="1"/>
-    <col min="28" max="28" width="25.5546875" customWidth="1"/>
-    <col min="29" max="1028" width="8.6640625" customWidth="1"/>
+    <col min="28" max="28" width="25.5703125" customWidth="1"/>
+    <col min="29" max="1028" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>2900615016094</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="2">
         <v>4562</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="Q2" s="5">
+      <c r="Q2" s="6">
         <v>931203</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="R2" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="S2" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="T2" s="6">
+      <c r="T2" s="7">
         <v>954.07</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="V2" s="1"/>
+      <c r="V2" s="8"/>
       <c r="W2" s="1"/>
       <c r="AB2" s="1"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>1901209018401</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="2">
         <v>8521</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="Q3" s="6">
         <v>931203</v>
       </c>
-      <c r="R3" s="6">
+      <c r="R3" s="7">
         <v>8907.56</v>
       </c>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="4" t="s">
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="5" t="s">
         <v>70</v>
       </c>
+      <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>1851220468624</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="2">
         <v>2156</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="Q4" s="6">
         <v>931203</v>
       </c>
-      <c r="R4" s="6">
+      <c r="R4" s="7">
         <v>4000</v>
       </c>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="4" t="s">
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="5" t="s">
         <v>71</v>
       </c>
+      <c r="V4" s="2"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>1910402069411</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="2">
         <v>1252</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="P5" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="2">
         <v>216103</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="R5" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="4" t="s">
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="5" t="s">
         <v>72</v>
       </c>
+      <c r="V5" s="2"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <v>2880226065884</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="2">
         <v>2315</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="O6" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="P6" s="4" t="s">
+      <c r="P6" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="2">
         <v>216103</v>
       </c>
-      <c r="R6" s="6">
+      <c r="R6" s="7">
         <v>10000</v>
       </c>
-      <c r="S6" s="6" t="s">
+      <c r="S6" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="T6" s="6">
+      <c r="T6" s="7">
         <v>1056.67</v>
       </c>
-      <c r="U6" s="4" t="s">
+      <c r="U6" s="5" t="s">
         <v>73</v>
       </c>
+      <c r="V6" s="2"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>2920917067140</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="2">
         <v>9856</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="O7" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="P7" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="2">
         <v>216103</v>
       </c>
-      <c r="R7" s="6">
+      <c r="R7" s="7">
         <v>15000</v>
       </c>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="4" t="s">
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="5" t="s">
         <v>74</v>
       </c>
+      <c r="V7" s="2"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <v>1920917358171</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="2">
         <v>7452</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="P8" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="2">
         <v>216103</v>
       </c>
-      <c r="R8" s="6">
+      <c r="R8" s="7">
         <v>15987.45</v>
       </c>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="4" t="s">
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="5" t="s">
         <v>93</v>
       </c>
+      <c r="V8" s="2"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="3">
         <v>1820929359776</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="2">
         <v>2380</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="O9" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="P9" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="2">
         <v>216103</v>
       </c>
-      <c r="R9" s="6">
+      <c r="R9" s="7">
         <v>15000</v>
       </c>
-      <c r="S9" s="6" t="s">
+      <c r="S9" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="T9" s="6"/>
-      <c r="U9" s="4" t="s">
+      <c r="T9" s="7"/>
+      <c r="U9" s="5" t="s">
         <v>94</v>
       </c>
+      <c r="V9" s="2"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="3">
         <v>2820929326615</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="2">
         <v>9431</v>
       </c>
-      <c r="O10" s="4" t="s">
+      <c r="O10" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="P10" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="2">
         <v>216103</v>
       </c>
-      <c r="R10" s="6">
+      <c r="R10" s="7">
         <v>19874.12</v>
       </c>
-      <c r="S10" s="6" t="s">
+      <c r="S10" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="T10" s="7" t="s">
+      <c r="T10" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="U10" s="4" t="s">
+      <c r="U10" s="5" t="s">
         <v>106</v>
       </c>
+      <c r="V10" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1653,22 +1663,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{260AF3CD-A374-47A7-A8E9-D4989E509984}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="50f7d85b-f98c-445e-b58e-72d6269df11c"/>
-    <ds:schemaRef ds:uri="2773402d-a253-4db6-8bd0-1165c16be02b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{260AF3CD-A374-47A7-A8E9-D4989E509984}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1678,8 +1673,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="eabad42a-89c6-42d5-ba30-2e7dff9f63a4"/>
     <ds:schemaRef ds:uri="2c4a328c-ab73-43c0-821c-f37f03fc26d5"/>
-    <ds:schemaRef ds:uri="2773402d-a253-4db6-8bd0-1165c16be02b"/>
-    <ds:schemaRef ds:uri="50f7d85b-f98c-445e-b58e-72d6269df11c"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>